<commit_message>
made some changes in component assignee script and correlation
</commit_message>
<xml_diff>
--- a/correlation/correlation.xlsx
+++ b/correlation/correlation.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,6 +410,11 @@
       <c r="K1" t="inlineStr">
         <is>
           <t>Reopened Percent</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Assignee Component</t>
         </is>
       </c>
     </row>
@@ -425,6 +430,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -472,6 +478,9 @@
       <c r="K3" t="n">
         <v>0</v>
       </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -519,6 +528,9 @@
       <c r="K4" t="n">
         <v>0</v>
       </c>
+      <c r="L4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -566,6 +578,9 @@
       <c r="K5" t="n">
         <v>4.580152671755725</v>
       </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -613,6 +628,9 @@
       <c r="K6" t="n">
         <v>7.920792079207921</v>
       </c>
+      <c r="L6" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -660,6 +678,9 @@
       <c r="K7" t="n">
         <v>8.163265306122449</v>
       </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -707,6 +728,9 @@
       <c r="K8" t="n">
         <v>3.846153846153846</v>
       </c>
+      <c r="L8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -754,6 +778,9 @@
       <c r="K9" t="n">
         <v>4.323458767013611</v>
       </c>
+      <c r="L9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -801,6 +828,9 @@
       <c r="K10" t="n">
         <v>0</v>
       </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -848,6 +878,9 @@
       <c r="K11" t="n">
         <v>2.352941176470588</v>
       </c>
+      <c r="L11" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -895,6 +928,9 @@
       <c r="K12" t="n">
         <v>1.092896174863388</v>
       </c>
+      <c r="L12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -942,6 +978,9 @@
       <c r="K13" t="n">
         <v>3.703703703703703</v>
       </c>
+      <c r="L13" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -989,6 +1028,9 @@
       <c r="K14" t="n">
         <v>1.333333333333333</v>
       </c>
+      <c r="L14" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1036,6 +1078,9 @@
       <c r="K15" t="n">
         <v>1.82370820668693</v>
       </c>
+      <c r="L15" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1083,6 +1128,9 @@
       <c r="K16" t="n">
         <v>0</v>
       </c>
+      <c r="L16" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1130,6 +1178,9 @@
       <c r="K17" t="n">
         <v>0</v>
       </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1177,6 +1228,9 @@
       <c r="K18" t="n">
         <v>0</v>
       </c>
+      <c r="L18" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1224,6 +1278,9 @@
       <c r="K19" t="n">
         <v>5.714285714285714</v>
       </c>
+      <c r="L19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1271,6 +1328,9 @@
       <c r="K20" t="n">
         <v>6.666666666666667</v>
       </c>
+      <c r="L20" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1318,6 +1378,9 @@
       <c r="K21" t="n">
         <v>6.896551724137931</v>
       </c>
+      <c r="L21" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1365,6 +1428,9 @@
       <c r="K22" t="n">
         <v>0</v>
       </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1412,6 +1478,9 @@
       <c r="K23" t="n">
         <v>0</v>
       </c>
+      <c r="L23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1459,6 +1528,9 @@
       <c r="K24" t="n">
         <v>6.666666666666667</v>
       </c>
+      <c r="L24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1506,6 +1578,9 @@
       <c r="K25" t="n">
         <v>7.84313725490196</v>
       </c>
+      <c r="L25" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1553,6 +1628,9 @@
       <c r="K26" t="n">
         <v>0</v>
       </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1600,6 +1678,9 @@
       <c r="K27" t="n">
         <v>0</v>
       </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1647,6 +1728,9 @@
       <c r="K28" t="n">
         <v>8.053691275167784</v>
       </c>
+      <c r="L28" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1694,6 +1778,9 @@
       <c r="K29" t="n">
         <v>0</v>
       </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1741,6 +1828,9 @@
       <c r="K30" t="n">
         <v>10.52631578947368</v>
       </c>
+      <c r="L30" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1788,6 +1878,9 @@
       <c r="K31" t="n">
         <v>0</v>
       </c>
+      <c r="L31" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1835,6 +1928,9 @@
       <c r="K32" t="n">
         <v>0</v>
       </c>
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1882,6 +1978,9 @@
       <c r="K33" t="n">
         <v>11.11111111111111</v>
       </c>
+      <c r="L33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1929,6 +2028,9 @@
       <c r="K34" t="n">
         <v>0</v>
       </c>
+      <c r="L34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1976,6 +2078,9 @@
       <c r="K35" t="n">
         <v>0</v>
       </c>
+      <c r="L35" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2023,6 +2128,9 @@
       <c r="K36" t="n">
         <v>2.73972602739726</v>
       </c>
+      <c r="L36" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2070,6 +2178,9 @@
       <c r="K37" t="n">
         <v>0</v>
       </c>
+      <c r="L37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2117,6 +2228,9 @@
       <c r="K38" t="n">
         <v>0</v>
       </c>
+      <c r="L38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2164,6 +2278,9 @@
       <c r="K39" t="n">
         <v>0</v>
       </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2211,6 +2328,9 @@
       <c r="K40" t="n">
         <v>0</v>
       </c>
+      <c r="L40" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2258,6 +2378,9 @@
       <c r="K41" t="n">
         <v>0</v>
       </c>
+      <c r="L41" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2305,6 +2428,9 @@
       <c r="K42" t="n">
         <v>0</v>
       </c>
+      <c r="L42" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2352,6 +2478,9 @@
       <c r="K43" t="n">
         <v>0</v>
       </c>
+      <c r="L43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2399,6 +2528,9 @@
       <c r="K44" t="n">
         <v>3.703703703703703</v>
       </c>
+      <c r="L44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2446,6 +2578,9 @@
       <c r="K45" t="n">
         <v>0</v>
       </c>
+      <c r="L45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2493,6 +2628,9 @@
       <c r="K46" t="n">
         <v>0</v>
       </c>
+      <c r="L46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2540,6 +2678,9 @@
       <c r="K47" t="n">
         <v>0</v>
       </c>
+      <c r="L47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2587,6 +2728,9 @@
       <c r="K48" t="n">
         <v>0</v>
       </c>
+      <c r="L48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2634,6 +2778,9 @@
       <c r="K49" t="n">
         <v>0</v>
       </c>
+      <c r="L49" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -2681,6 +2828,9 @@
       <c r="K50" t="n">
         <v>0</v>
       </c>
+      <c r="L50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2728,6 +2878,9 @@
       <c r="K51" t="n">
         <v>0</v>
       </c>
+      <c r="L51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2775,6 +2928,9 @@
       <c r="K52" t="n">
         <v>0</v>
       </c>
+      <c r="L52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -2822,6 +2978,9 @@
       <c r="K53" t="n">
         <v>11.76470588235294</v>
       </c>
+      <c r="L53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -2869,6 +3028,9 @@
       <c r="K54" t="n">
         <v>33.33333333333333</v>
       </c>
+      <c r="L54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2916,6 +3078,9 @@
       <c r="K55" t="n">
         <v>0</v>
       </c>
+      <c r="L55" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2963,6 +3128,9 @@
       <c r="K56" t="n">
         <v>7.692307692307693</v>
       </c>
+      <c r="L56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -3010,6 +3178,9 @@
       <c r="K57" t="n">
         <v>9.45945945945946</v>
       </c>
+      <c r="L57" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -3057,6 +3228,9 @@
       <c r="K58" t="n">
         <v>0</v>
       </c>
+      <c r="L58" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -3104,6 +3278,9 @@
       <c r="K59" t="n">
         <v>16.66666666666666</v>
       </c>
+      <c r="L59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -3151,6 +3328,9 @@
       <c r="K60" t="n">
         <v>11.96581196581197</v>
       </c>
+      <c r="L60" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -3198,6 +3378,9 @@
       <c r="K61" t="n">
         <v>25</v>
       </c>
+      <c r="L61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3245,6 +3428,9 @@
       <c r="K62" t="n">
         <v>4.081632653061225</v>
       </c>
+      <c r="L62" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -3292,6 +3478,9 @@
       <c r="K63" t="n">
         <v>14.28571428571428</v>
       </c>
+      <c r="L63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3339,6 +3528,9 @@
       <c r="K64" t="n">
         <v>0</v>
       </c>
+      <c r="L64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -3386,6 +3578,9 @@
       <c r="K65" t="n">
         <v>0</v>
       </c>
+      <c r="L65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3433,6 +3628,9 @@
       <c r="K66" t="n">
         <v>0</v>
       </c>
+      <c r="L66" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -3480,6 +3678,9 @@
       <c r="K67" t="n">
         <v>0</v>
       </c>
+      <c r="L67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -3527,6 +3728,9 @@
       <c r="K68" t="n">
         <v>0</v>
       </c>
+      <c r="L68" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -3574,6 +3778,9 @@
       <c r="K69" t="n">
         <v>0</v>
       </c>
+      <c r="L69" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3621,6 +3828,9 @@
       <c r="K70" t="n">
         <v>0</v>
       </c>
+      <c r="L70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -3668,6 +3878,9 @@
       <c r="K71" t="n">
         <v>0</v>
       </c>
+      <c r="L71" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -3715,6 +3928,9 @@
       <c r="K72" t="n">
         <v>0</v>
       </c>
+      <c r="L72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -3762,6 +3978,9 @@
       <c r="K73" t="n">
         <v>0</v>
       </c>
+      <c r="L73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -3809,6 +4028,9 @@
       <c r="K74" t="n">
         <v>1.526717557251908</v>
       </c>
+      <c r="L74" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -3856,6 +4078,9 @@
       <c r="K75" t="n">
         <v>0</v>
       </c>
+      <c r="L75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -3903,6 +4128,9 @@
       <c r="K76" t="n">
         <v>12.5</v>
       </c>
+      <c r="L76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -3950,6 +4178,9 @@
       <c r="K77" t="n">
         <v>0</v>
       </c>
+      <c r="L77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -3997,6 +4228,9 @@
       <c r="K78" t="n">
         <v>0</v>
       </c>
+      <c r="L78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -4044,6 +4278,9 @@
       <c r="K79" t="n">
         <v>0</v>
       </c>
+      <c r="L79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -4091,6 +4328,9 @@
       <c r="K80" t="n">
         <v>0</v>
       </c>
+      <c r="L80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -4138,6 +4378,9 @@
       <c r="K81" t="n">
         <v>0</v>
       </c>
+      <c r="L81" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -4185,6 +4428,9 @@
       <c r="K82" t="n">
         <v>0</v>
       </c>
+      <c r="L82" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -4232,6 +4478,9 @@
       <c r="K83" t="n">
         <v>0</v>
       </c>
+      <c r="L83" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -4279,6 +4528,9 @@
       <c r="K84" t="n">
         <v>0</v>
       </c>
+      <c r="L84" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -4326,6 +4578,9 @@
       <c r="K85" t="n">
         <v>0</v>
       </c>
+      <c r="L85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -4373,6 +4628,9 @@
       <c r="K86" t="n">
         <v>0</v>
       </c>
+      <c r="L86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -4420,6 +4678,9 @@
       <c r="K87" t="n">
         <v>0.9615384615384616</v>
       </c>
+      <c r="L87" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -4467,6 +4728,9 @@
       <c r="K88" t="n">
         <v>7.61904761904762</v>
       </c>
+      <c r="L88" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -4514,6 +4778,9 @@
       <c r="K89" t="n">
         <v>0</v>
       </c>
+      <c r="L89" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4561,6 +4828,9 @@
       <c r="K90" t="n">
         <v>5.179282868525896</v>
       </c>
+      <c r="L90" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -4608,6 +4878,9 @@
       <c r="K91" t="n">
         <v>0</v>
       </c>
+      <c r="L91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -4655,6 +4928,9 @@
       <c r="K92" t="n">
         <v>7.741935483870968</v>
       </c>
+      <c r="L92" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -4702,6 +4978,9 @@
       <c r="K93" t="n">
         <v>9.090909090909092</v>
       </c>
+      <c r="L93" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -4749,6 +5028,9 @@
       <c r="K94" t="n">
         <v>0</v>
       </c>
+      <c r="L94" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -4796,6 +5078,9 @@
       <c r="K95" t="n">
         <v>0</v>
       </c>
+      <c r="L95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -4843,6 +5128,9 @@
       <c r="K96" t="n">
         <v>7.84313725490196</v>
       </c>
+      <c r="L96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -4890,6 +5178,9 @@
       <c r="K97" t="n">
         <v>0</v>
       </c>
+      <c r="L97" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -4937,6 +5228,9 @@
       <c r="K98" t="n">
         <v>4.651162790697675</v>
       </c>
+      <c r="L98" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -4984,6 +5278,9 @@
       <c r="K99" t="n">
         <v>0</v>
       </c>
+      <c r="L99" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -5031,6 +5328,9 @@
       <c r="K100" t="n">
         <v>0</v>
       </c>
+      <c r="L100" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -5078,6 +5378,9 @@
       <c r="K101" t="n">
         <v>2.325581395348837</v>
       </c>
+      <c r="L101" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -5125,6 +5428,9 @@
       <c r="K102" t="n">
         <v>7.692307692307693</v>
       </c>
+      <c r="L102" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -5172,6 +5478,9 @@
       <c r="K103" t="n">
         <v>12.5</v>
       </c>
+      <c r="L103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -5219,6 +5528,9 @@
       <c r="K104" t="n">
         <v>0</v>
       </c>
+      <c r="L104" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -5266,6 +5578,9 @@
       <c r="K105" t="n">
         <v>10</v>
       </c>
+      <c r="L105" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -5313,6 +5628,9 @@
       <c r="K106" t="n">
         <v>0</v>
       </c>
+      <c r="L106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -5360,6 +5678,9 @@
       <c r="K107" t="n">
         <v>0</v>
       </c>
+      <c r="L107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -5407,6 +5728,9 @@
       <c r="K108" t="n">
         <v>0</v>
       </c>
+      <c r="L108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -5454,6 +5778,9 @@
       <c r="K109" t="n">
         <v>0</v>
       </c>
+      <c r="L109" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -5501,6 +5828,9 @@
       <c r="K110" t="n">
         <v>0</v>
       </c>
+      <c r="L110" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -5548,6 +5878,9 @@
       <c r="K111" t="n">
         <v>0</v>
       </c>
+      <c r="L111" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5595,6 +5928,9 @@
       <c r="K112" t="n">
         <v>0</v>
       </c>
+      <c r="L112" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -5642,6 +5978,9 @@
       <c r="K113" t="n">
         <v>0</v>
       </c>
+      <c r="L113" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -5689,6 +6028,9 @@
       <c r="K114" t="n">
         <v>0</v>
       </c>
+      <c r="L114" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -5736,6 +6078,9 @@
       <c r="K115" t="n">
         <v>0</v>
       </c>
+      <c r="L115" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -5783,6 +6128,9 @@
       <c r="K116" t="n">
         <v>0</v>
       </c>
+      <c r="L116" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -5830,6 +6178,9 @@
       <c r="K117" t="n">
         <v>3.571428571428571</v>
       </c>
+      <c r="L117" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -5877,6 +6228,9 @@
       <c r="K118" t="n">
         <v>0</v>
       </c>
+      <c r="L118" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -5924,6 +6278,9 @@
       <c r="K119" t="n">
         <v>0</v>
       </c>
+      <c r="L119" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -5971,6 +6328,9 @@
       <c r="K120" t="n">
         <v>18.18181818181818</v>
       </c>
+      <c r="L120" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -6018,6 +6378,9 @@
       <c r="K121" t="n">
         <v>0</v>
       </c>
+      <c r="L121" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -6065,6 +6428,9 @@
       <c r="K122" t="n">
         <v>2.857142857142857</v>
       </c>
+      <c r="L122" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -6112,6 +6478,9 @@
       <c r="K123" t="n">
         <v>0</v>
       </c>
+      <c r="L123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -6159,6 +6528,9 @@
       <c r="K124" t="n">
         <v>0</v>
       </c>
+      <c r="L124" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -6206,6 +6578,9 @@
       <c r="K125" t="n">
         <v>0</v>
       </c>
+      <c r="L125" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -6253,6 +6628,9 @@
       <c r="K126" t="n">
         <v>0</v>
       </c>
+      <c r="L126" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -6300,6 +6678,9 @@
       <c r="K127" t="n">
         <v>11.11111111111111</v>
       </c>
+      <c r="L127" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -6347,6 +6728,9 @@
       <c r="K128" t="n">
         <v>0</v>
       </c>
+      <c r="L128" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -6393,6 +6777,9 @@
       </c>
       <c r="K129" t="n">
         <v>0</v>
+      </c>
+      <c r="L129" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>